<commit_message>
update of role interaction part I
1. commander would scan other minor charactors.
2. SWAT would supply nearby characters.
</commit_message>
<xml_diff>
--- a/技能間互動.xlsx
+++ b/技能間互動.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Hsu\Documents\GitHub\CS1.6-LeaderMode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E302F8FA-0F8B-4102-A361-23EAB8D50175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6060B4-2BEC-47C1-9B41-2D9A2801ECE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DD489BB-1039-421B-BD99-6627FF7F1155}"/>
+    <workbookView xWindow="12885" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{4DD489BB-1039-421B-BD99-6627FF7F1155}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,10 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>治療彈可以撤銷冰雷</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>神射使用技能時，爆頭強制擊殺暴徒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>治療彈撤銷絕唱但不致其於死地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>治療彈範圍內毒氣與電擊無效；治療飛鏢治癒毒氣、電擊</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -125,10 +117,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>火焰中止治療彈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>教父技能作用下無法隱身</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>教父技能作用時無法絕唱，若在絕唱中則中止之。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火焰中止治療煙霧彈，治療飛鏢可以解除燃燒狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>治療煙霧(治療飛鏢同)彈撤銷絕唱但不致其於死地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>治療煙霧(治療飛鏢同)彈可以撤銷冰雷</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -558,7 +558,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -654,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -706,13 +706,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -772,13 +772,13 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -805,10 +805,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>10</v>
@@ -840,19 +840,19 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -877,22 +877,22 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="1"/>

</xml_diff>